<commit_message>
changed forward-backslashes to hopefully fix os.walk issue on pi
</commit_message>
<xml_diff>
--- a/data/parameter_list.xlsx
+++ b/data/parameter_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Spring_2025\Team_Projects_II\repo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7A37B8-98CE-4F06-A2EF-7D30F6F733B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032E1A2A-AF05-445B-A411-E387DBCAA828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,12 +127,6 @@
     <t>elapsed_time</t>
   </si>
   <si>
-    <t>..\assets\test_cases\test_case21.245\train\</t>
-  </si>
-  <si>
-    <t>..\assets\test_cases\test_case21.245\test\</t>
-  </si>
-  <si>
     <t>128, 128</t>
   </si>
   <si>
@@ -158,6 +152,12 @@
   </si>
   <si>
     <t>0, 256, 0, 256, 0, 256</t>
+  </si>
+  <si>
+    <t>../assets/test_cases/test_case21.245/train/</t>
+  </si>
+  <si>
+    <t>../assets/test_cases/test_case21.245/test/</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -638,10 +640,10 @@
         <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -659,25 +661,25 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>40</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>41</v>
-      </c>
-      <c r="N2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2" t="s">
-        <v>43</v>
       </c>
       <c r="P2">
         <v>2</v>
@@ -704,10 +706,10 @@
         <v>8</v>
       </c>
       <c r="X2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Y2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Z2">
         <v>500</v>
@@ -737,7 +739,7 @@
         <v>96.4</v>
       </c>
       <c r="AI2">
-        <v>50.96</v>
+        <v>49.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>